<commit_message>
Attached uploading of inventory and users to main form
</commit_message>
<xml_diff>
--- a/UserUploadFormat.xlsx
+++ b/UserUploadFormat.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathaniel Angelico\Desktop\ANS-SEIS-TV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A39B2E3-53B3-4FF0-881F-35E60C1AE9D0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA0CE90C-4A7B-4232-A4E7-AD9719A3981B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{B55A943C-7D57-4CFE-A143-E7E9D1BE715A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
   <si>
     <t>Username</t>
   </si>
@@ -45,40 +45,13 @@
     <t>UsertypeID</t>
   </si>
   <si>
-    <t>Person1</t>
-  </si>
-  <si>
-    <t>Person2</t>
-  </si>
-  <si>
-    <t>Person3</t>
-  </si>
-  <si>
-    <t>NameName1</t>
-  </si>
-  <si>
-    <t>NameName2</t>
-  </si>
-  <si>
-    <t>NameName3</t>
-  </si>
-  <si>
-    <t>NameN1</t>
-  </si>
-  <si>
-    <t>NameN2</t>
-  </si>
-  <si>
-    <t>NameN3</t>
-  </si>
-  <si>
-    <t>Last1</t>
-  </si>
-  <si>
-    <t>Last2</t>
-  </si>
-  <si>
-    <t>Last3</t>
+    <t>User1</t>
+  </si>
+  <si>
+    <t>User2</t>
+  </si>
+  <si>
+    <t>User3</t>
   </si>
 </sst>
 </file>
@@ -439,7 +412,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D4"/>
+      <selection activeCell="A2" sqref="A2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,13 +445,13 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E2" s="2">
         <v>9395686461</v>
@@ -492,13 +465,13 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E3" s="2">
         <v>9222729916</v>
@@ -512,13 +485,13 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="E4" s="2">
         <v>3123456789</v>

</xml_diff>